<commit_message>
performance improvements and updated warehouses
</commit_message>
<xml_diff>
--- a/templates/API_MMS010MI_AddLocation.xlsx
+++ b/templates/API_MMS010MI_AddLocation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BradHarrison\PycharmProjects\m3DataConversion\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bharrison\PycharmProjects\m3DataConversion\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C882711-7EC0-49F5-98B8-23D070B8D94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FB659A-BE88-4DF5-9368-561232F5F454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="1680" windowWidth="38325" windowHeight="18660" xr2:uid="{773610F9-17C7-4B99-9DF2-680F2E09EA34}"/>
+    <workbookView xWindow="8265" yWindow="2790" windowWidth="48195" windowHeight="18090" xr2:uid="{773610F9-17C7-4B99-9DF2-680F2E09EA34}"/>
   </bookViews>
   <sheets>
     <sheet name="API_MMS010MI_AddLocation" sheetId="2" r:id="rId1"/>
@@ -1739,7 +1739,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="99">
   <si>
     <t>MESSAGE</t>
   </si>
@@ -2034,6 +2034,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>yes|Opt:T/U/B</t>
   </si>
 </sst>
 </file>
@@ -2450,7 +2453,7 @@
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AW13" sqref="AW13"/>
+      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,13 +2767,13 @@
         <v>97</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>97</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>97</v>
@@ -2791,7 +2794,7 @@
         <v>97</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>2</v>
@@ -2842,7 +2845,7 @@
         <v>97</v>
       </c>
       <c r="AE3" s="6" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="AF3" s="6" t="s">
         <v>2</v>

</xml_diff>